<commit_message>
add week 5 data
</commit_message>
<xml_diff>
--- a/Vaccine-surveillance-report-week-4_COVID_vacc_death_raw_data.xlsx
+++ b/Vaccine-surveillance-report-week-4_COVID_vacc_death_raw_data.xlsx
@@ -5,20 +5,23 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\COVID_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15708" windowHeight="8016" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8028" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="diag" sheetId="1" r:id="rId1"/>
-    <sheet name="death28" sheetId="2" r:id="rId2"/>
-    <sheet name="death60" sheetId="3" r:id="rId3"/>
+    <sheet name="diag_week_4" sheetId="1" r:id="rId1"/>
+    <sheet name="death28_week_4" sheetId="2" r:id="rId2"/>
+    <sheet name="death60_week_4" sheetId="3" r:id="rId3"/>
+    <sheet name="diag_week_5" sheetId="4" r:id="rId4"/>
+    <sheet name="death28_week_5" sheetId="5" r:id="rId5"/>
+    <sheet name="death_week_5" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_ftn1" localSheetId="1">death28!#REF!</definedName>
-    <definedName name="_ftnref1" localSheetId="1">death28!#REF!</definedName>
+    <definedName name="_ftn1" localSheetId="1">death28_week_4!#REF!</definedName>
+    <definedName name="_ftnref1" localSheetId="1">death28_week_4!#REF!</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="51">
   <si>
     <t>Cases reported by specimen date between week 52 2021 (w/e 02/01/2022) and week 3</t>
   </si>
@@ -140,6 +143,63 @@
   </si>
   <si>
     <t>Received one dose, ≥21 days before specimen date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Received one dose (1 to 20 days before specimen date) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cases reported by specimen date between week 1 2022 (w/e 09/01/2022) and week 4 2022 (w/e 30/01/2022) </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Received one dose, ≥21 days before specimen date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Second dose ≥14 days before specimen date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Third dose ≥14 days before specimen date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Received one dose, ≥21 days before specimen date </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">[1] </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Third dose ≥14 days before specimen date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Death within 28 days of positive COVID-19 test by date of death between week 1 2022 (w/e 09/01/2022) and week 4 2022 (w/e 30/01/2022) </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Death within 60 days of positive COVID-19 test by date of death between week 1 2022 (w/e 09/01/2022) and week 4 2022 (w/e 30/01/2022) </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Received one dose (1 to 20 days before specimen date) </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Received one dose, ≥21 days before specimen date </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Second dose ≥14 days before specimen date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -185,12 +245,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -475,7 +538,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -483,29 +546,29 @@
     <col min="1" max="1" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="113.4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -989,7 +1052,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -1241,4 +1304,777 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="8" width="18.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="64.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="2">
+        <v>814347</v>
+      </c>
+      <c r="C2" s="2">
+        <v>46904</v>
+      </c>
+      <c r="D2" s="2">
+        <v>612529</v>
+      </c>
+      <c r="E2" s="2">
+        <v>8151</v>
+      </c>
+      <c r="F2" s="2">
+        <v>121434</v>
+      </c>
+      <c r="G2" s="2">
+        <v>24018</v>
+      </c>
+      <c r="H2" s="2">
+        <v>1311</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="2">
+        <v>512080</v>
+      </c>
+      <c r="C3" s="2">
+        <v>46298</v>
+      </c>
+      <c r="D3" s="2">
+        <v>91944</v>
+      </c>
+      <c r="E3" s="2">
+        <v>4387</v>
+      </c>
+      <c r="F3" s="2">
+        <v>30908</v>
+      </c>
+      <c r="G3" s="2">
+        <v>217861</v>
+      </c>
+      <c r="H3" s="2">
+        <v>120682</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="2">
+        <v>523577</v>
+      </c>
+      <c r="C4" s="2">
+        <v>37348</v>
+      </c>
+      <c r="D4" s="2">
+        <v>76644</v>
+      </c>
+      <c r="E4" s="2">
+        <v>2583</v>
+      </c>
+      <c r="F4" s="2">
+        <v>20293</v>
+      </c>
+      <c r="G4" s="2">
+        <v>182366</v>
+      </c>
+      <c r="H4" s="2">
+        <v>204343</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="2">
+        <v>421265</v>
+      </c>
+      <c r="C5" s="2">
+        <v>25690</v>
+      </c>
+      <c r="D5" s="2">
+        <v>37245</v>
+      </c>
+      <c r="E5">
+        <v>979</v>
+      </c>
+      <c r="F5" s="2">
+        <v>9522</v>
+      </c>
+      <c r="G5" s="2">
+        <v>108733</v>
+      </c>
+      <c r="H5" s="2">
+        <v>239096</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="2">
+        <v>302201</v>
+      </c>
+      <c r="C6" s="2">
+        <v>17986</v>
+      </c>
+      <c r="D6" s="2">
+        <v>16507</v>
+      </c>
+      <c r="E6">
+        <v>392</v>
+      </c>
+      <c r="F6" s="2">
+        <v>3922</v>
+      </c>
+      <c r="G6" s="2">
+        <v>50303</v>
+      </c>
+      <c r="H6" s="2">
+        <v>213091</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="2">
+        <v>160768</v>
+      </c>
+      <c r="C7" s="2">
+        <v>10026</v>
+      </c>
+      <c r="D7" s="2">
+        <v>5915</v>
+      </c>
+      <c r="E7">
+        <v>160</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1395</v>
+      </c>
+      <c r="G7" s="2">
+        <v>14724</v>
+      </c>
+      <c r="H7" s="2">
+        <v>128548</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="2">
+        <v>82218</v>
+      </c>
+      <c r="C8" s="2">
+        <v>5409</v>
+      </c>
+      <c r="D8" s="2">
+        <v>2032</v>
+      </c>
+      <c r="E8">
+        <v>68</v>
+      </c>
+      <c r="F8">
+        <v>589</v>
+      </c>
+      <c r="G8" s="2">
+        <v>4415</v>
+      </c>
+      <c r="H8" s="2">
+        <v>69705</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="2">
+        <v>55621</v>
+      </c>
+      <c r="C9" s="2">
+        <v>5809</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1463</v>
+      </c>
+      <c r="E9">
+        <v>28</v>
+      </c>
+      <c r="F9">
+        <v>576</v>
+      </c>
+      <c r="G9" s="2">
+        <v>4911</v>
+      </c>
+      <c r="H9" s="2">
+        <v>42834</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A2:A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="8" width="23.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="97.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3">
+        <v>12</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>8</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4">
+        <v>31</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>16</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>9</v>
+      </c>
+      <c r="H4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5">
+        <v>76</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>30</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>6</v>
+      </c>
+      <c r="G5">
+        <v>30</v>
+      </c>
+      <c r="H5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6">
+        <v>125</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>49</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>13</v>
+      </c>
+      <c r="G6">
+        <v>38</v>
+      </c>
+      <c r="H6">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7">
+        <v>311</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>106</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>21</v>
+      </c>
+      <c r="G7">
+        <v>115</v>
+      </c>
+      <c r="H7">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8">
+        <v>642</v>
+      </c>
+      <c r="C8">
+        <v>12</v>
+      </c>
+      <c r="D8">
+        <v>192</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>21</v>
+      </c>
+      <c r="G8">
+        <v>227</v>
+      </c>
+      <c r="H8">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9">
+        <v>1220</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>241</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <v>51</v>
+      </c>
+      <c r="G9">
+        <v>372</v>
+      </c>
+      <c r="H9">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="2">
+        <v>3137</v>
+      </c>
+      <c r="C10">
+        <v>16</v>
+      </c>
+      <c r="D10">
+        <v>373</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="F10">
+        <v>89</v>
+      </c>
+      <c r="G10">
+        <v>910</v>
+      </c>
+      <c r="H10" s="2">
+        <v>1744</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="8" width="18.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>13</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3">
+        <v>45</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>25</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>13</v>
+      </c>
+      <c r="H3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4">
+        <v>102</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>43</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>9</v>
+      </c>
+      <c r="G4">
+        <v>36</v>
+      </c>
+      <c r="H4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5">
+        <v>159</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>64</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>14</v>
+      </c>
+      <c r="G5">
+        <v>49</v>
+      </c>
+      <c r="H5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6">
+        <v>407</v>
+      </c>
+      <c r="C6">
+        <v>9</v>
+      </c>
+      <c r="D6">
+        <v>139</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>29</v>
+      </c>
+      <c r="G6">
+        <v>146</v>
+      </c>
+      <c r="H6">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7">
+        <v>775</v>
+      </c>
+      <c r="C7">
+        <v>13</v>
+      </c>
+      <c r="D7">
+        <v>234</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>23</v>
+      </c>
+      <c r="G7">
+        <v>276</v>
+      </c>
+      <c r="H7">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8">
+        <v>1427</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>268</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8">
+        <v>60</v>
+      </c>
+      <c r="G8">
+        <v>453</v>
+      </c>
+      <c r="H8">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="2">
+        <v>3555</v>
+      </c>
+      <c r="C9">
+        <v>18</v>
+      </c>
+      <c r="D9">
+        <v>395</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <v>97</v>
+      </c>
+      <c r="G9" s="2">
+        <v>1081</v>
+      </c>
+      <c r="H9" s="2">
+        <v>1959</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add week 5 data and render format
</commit_message>
<xml_diff>
--- a/Vaccine-surveillance-report-week-4_COVID_vacc_death_raw_data.xlsx
+++ b/Vaccine-surveillance-report-week-4_COVID_vacc_death_raw_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8028" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="6732" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="diag_week_4" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="50">
   <si>
     <t>Cases reported by specimen date between week 52 2021 (w/e 02/01/2022) and week 3</t>
   </si>
@@ -171,10 +171,6 @@
   </si>
   <si>
     <t xml:space="preserve">Received one dose, ≥21 days before specimen date </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">[1] </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1310,7 +1306,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
@@ -1319,7 +1315,7 @@
     <col min="1" max="8" width="18.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="64.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="97.2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
@@ -1562,10 +1558,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A2:A3"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -1575,7 +1571,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="97.2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>16</v>
@@ -1596,222 +1592,214 @@
         <v>41</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="G2" t="s">
-        <v>44</v>
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>12</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>8</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B3">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B4">
-        <v>31</v>
+        <v>76</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G4">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="H4">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B5">
-        <v>76</v>
+        <v>125</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="G5">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="H5">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B6">
-        <v>125</v>
+        <v>311</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D6">
-        <v>49</v>
+        <v>106</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="G6">
-        <v>38</v>
+        <v>115</v>
       </c>
       <c r="H6">
-        <v>24</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B7">
-        <v>311</v>
+        <v>642</v>
       </c>
       <c r="C7">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D7">
-        <v>106</v>
+        <v>192</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7">
         <v>21</v>
       </c>
       <c r="G7">
-        <v>115</v>
+        <v>227</v>
       </c>
       <c r="H7">
-        <v>65</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B8">
-        <v>642</v>
+        <v>1220</v>
       </c>
       <c r="C8">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D8">
-        <v>192</v>
+        <v>241</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F8">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="G8">
-        <v>227</v>
+        <v>372</v>
       </c>
       <c r="H8">
-        <v>189</v>
+        <v>549</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9">
-        <v>1220</v>
+        <v>27</v>
+      </c>
+      <c r="B9" s="2">
+        <v>3137</v>
       </c>
       <c r="C9">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D9">
-        <v>241</v>
+        <v>373</v>
       </c>
       <c r="E9">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F9">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="G9">
-        <v>372</v>
-      </c>
-      <c r="H9">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="2">
-        <v>3137</v>
-      </c>
-      <c r="C10">
-        <v>16</v>
-      </c>
-      <c r="D10">
-        <v>373</v>
-      </c>
-      <c r="E10">
-        <v>5</v>
-      </c>
-      <c r="F10">
-        <v>89</v>
-      </c>
-      <c r="G10">
         <v>910</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H9" s="2">
         <v>1744</v>
       </c>
     </row>
@@ -1825,7 +1813,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -1836,7 +1824,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>16</v>
@@ -1848,16 +1836,16 @@
         <v>18</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>